<commit_message>
added excel data read method
</commit_message>
<xml_diff>
--- a/src/TestData/TestData.xlsx
+++ b/src/TestData/TestData.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgajul\eclipse-workspace\SeleniumPractise\src\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CCCC186-3CA2-4532-A2CE-7853B2742682}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BF2B52F0-A414-4816-8D5B-8413E5AA03F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" xr2:uid="{C2A3BAE7-E1E7-4439-BA8B-C8B535EC51A6}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14460" windowHeight="10940" xr2:uid="{C2A3BAE7-E1E7-4439-BA8B-C8B535EC51A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -52,6 +57,15 @@
   </si>
   <si>
     <t>ravi@yahoo.com</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -414,19 +428,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1027CB0-902A-4970-8B22-4FCDA40209D0}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +451,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -447,8 +471,17 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D2">
+        <v>9052046524</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2">
+        <v>12.34</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -457,6 +490,15 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D3">
+        <v>9076565434</v>
+      </c>
+      <c r="E3">
+        <v>56456464</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>